<commit_message>
Working on Lab 3
</commit_message>
<xml_diff>
--- a/Proiecte grupa 244.xlsx
+++ b/Proiecte grupa 244.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npaslaru\OneDrive - ENDAVA\Documents\Personal\Facultate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npaslaru\IdeaProjects\PAO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C31DDD4-399E-47E6-BC89-32ECD16833E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22493306-9E29-47E3-8E64-7468956738C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59617D52-F6F5-4272-AFD7-E5ADEA2B3857}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="161">
   <si>
     <t>Proiect</t>
   </si>
@@ -422,9 +422,6 @@
     <t>458/2021</t>
   </si>
   <si>
-    <t xml:space="preserve">mircea.popescu6@s.unibuc.ro </t>
-  </si>
-  <si>
     <t>POPESCU</t>
   </si>
   <si>
@@ -509,20 +506,26 @@
     <t>Vola.ro</t>
   </si>
   <si>
-    <t>YYY</t>
-  </si>
-  <si>
     <t>Turneu Sah</t>
   </si>
   <si>
     <t>Echipa</t>
+  </si>
+  <si>
+    <t>Dumbrava Minunata</t>
+  </si>
+  <si>
+    <t>Scoala</t>
+  </si>
+  <si>
+    <t>mircea.popescu@s.unibuc.ro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,6 +547,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -611,10 +622,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -622,9 +634,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -644,58 +653,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -939,6 +906,53 @@
         </left>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -953,16 +967,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8AA3949-15D7-4501-8E64-1B8874B8297F}" name="Table1" displayName="Table1" ref="A4:I31" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8AA3949-15D7-4501-8E64-1B8874B8297F}" name="Table1" displayName="Table1" ref="A4:I31" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A4:I31" xr:uid="{E8AA3949-15D7-4501-8E64-1B8874B8297F}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{CCDAC79D-91C4-481F-B5AB-7340F59F7B3B}" name="Nr. crt. " dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{6269DEFC-7906-4B42-A96A-59DE0D4F9B41}" name="Nr. matricol" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{8F25FE3B-5EAA-47AD-B377-DF2223E2E738}" name="Grupa" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{4EC44123-9DDC-4B8C-9A53-8B3B0714956C}" name="Adresa intitutionala " dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{F9B606ED-C2BA-4082-9258-F84C7504B9C5}" name="Nume" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{703EEE7A-1420-4340-BC47-3BAFAEE610D1}" name="Initiala tata" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{2D0C8BAD-2927-4F69-9099-A283227D77FC}" name="Prenume" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{CCDAC79D-91C4-481F-B5AB-7340F59F7B3B}" name="Nr. crt. " dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{6269DEFC-7906-4B42-A96A-59DE0D4F9B41}" name="Nr. matricol" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{8F25FE3B-5EAA-47AD-B377-DF2223E2E738}" name="Grupa" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{4EC44123-9DDC-4B8C-9A53-8B3B0714956C}" name="Adresa intitutionala " dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{F9B606ED-C2BA-4082-9258-F84C7504B9C5}" name="Nume" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{703EEE7A-1420-4340-BC47-3BAFAEE610D1}" name="Initiala tata" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{2D0C8BAD-2927-4F69-9099-A283227D77FC}" name="Prenume" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{0BD08CA3-4AA0-430B-A4ED-3C225BBB0FE0}" name="Echipa"/>
     <tableColumn id="9" xr3:uid="{5514531E-6714-4584-8B18-78EFF6CAA5D1}" name="Proiect"/>
   </tableColumns>
@@ -1267,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF0F1FF-3AF6-4B0C-9230-C0193D72F887}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1282,17 +1296,17 @@
     <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1316,7 +1330,7 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1337,15 +1351,15 @@
       <c r="G4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="I4" s="8" t="s">
+      <c r="H4" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1366,15 +1380,15 @@
       <c r="G5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>158</v>
+      <c r="I5" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1395,15 +1409,15 @@
       <c r="G6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1424,15 +1438,15 @@
       <c r="G7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="H7" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1453,15 +1467,15 @@
       <c r="G8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1482,15 +1496,15 @@
       <c r="G9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1511,15 +1525,15 @@
       <c r="G10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1540,15 +1554,15 @@
       <c r="G11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1571,7 +1585,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1594,7 +1608,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1615,15 +1629,15 @@
       <c r="G14" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1644,15 +1658,15 @@
       <c r="G15" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>156</v>
+      <c r="I15" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1674,8 +1688,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1696,15 +1710,15 @@
       <c r="G17" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="9">
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1725,15 +1739,15 @@
       <c r="G18" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="9">
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1754,15 +1768,15 @@
       <c r="G19" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+      <c r="I19" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="9">
         <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1784,8 +1798,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="9">
         <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1806,15 +1820,15 @@
       <c r="G21" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="9">
         <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1835,15 +1849,15 @@
       <c r="G22" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="9">
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1864,12 +1878,15 @@
       <c r="G23" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H23" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="10">
+      <c r="H23" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="9">
         <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1890,15 +1907,15 @@
       <c r="G24" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="10">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="9">
         <v>21</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1919,15 +1936,16 @@
       <c r="G25" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="10">
+      <c r="I25" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="9">
         <v>22</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1937,167 +1955,173 @@
         <v>244</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="9">
+        <v>23</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="10">
-        <v>23</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="C27" s="3">
         <v>244</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G27" s="3" t="s">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="9">
+        <v>24</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="10">
-        <v>24</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3">
+        <v>244</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C28" s="3">
-        <v>244</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="H28" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="9">
+        <v>25</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="H28" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="10">
-        <v>25</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3">
+        <v>244</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C29" s="3">
-        <v>244</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="H29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="9">
+        <v>26</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="10">
-        <v>26</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3">
+        <v>244</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C30" s="3">
-        <v>244</v>
-      </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>82</v>
       </c>
       <c r="G30" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="9">
+        <v>27</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="H30" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="10">
-        <v>27</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3">
+        <v>244</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C31" s="3">
-        <v>244</v>
-      </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>157</v>
+      <c r="H31" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I31" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D27" r:id="rId1" xr:uid="{05A61D33-4089-40B2-8C6C-F3386C8C4755}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>